<commit_message>
08-01-2025 upload a file
</commit_message>
<xml_diff>
--- a/Daily_Tasks.xlsx
+++ b/Daily_Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daily_Status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE9294A-44C0-4412-A4FA-F65CA0E2EEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F87BEA-9BCD-457A-836F-B8ED0968E281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="70">
   <si>
     <t>S.NO</t>
   </si>
@@ -313,16 +313,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -605,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T72"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +617,7 @@
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="57.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="55.77734375" customWidth="1"/>
+    <col min="5" max="5" width="89.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -641,7 +641,7 @@
       <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="13">
         <v>45635</v>
       </c>
       <c r="C2" t="s">
@@ -653,7 +653,7 @@
     </row>
     <row r="3" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
-      <c r="B3" s="15"/>
+      <c r="B3" s="13"/>
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -663,7 +663,7 @@
     </row>
     <row r="4" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
-      <c r="B4" s="15"/>
+      <c r="B4" s="13"/>
       <c r="C4" t="s">
         <v>7</v>
       </c>
@@ -673,7 +673,7 @@
     </row>
     <row r="5" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
-      <c r="B5" s="15"/>
+      <c r="B5" s="13"/>
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -685,7 +685,7 @@
     </row>
     <row r="6" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
-      <c r="B6" s="15"/>
+      <c r="B6" s="13"/>
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -695,7 +695,7 @@
     </row>
     <row r="7" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
-      <c r="B7" s="15"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
@@ -707,7 +707,7 @@
       <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>45636</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -719,7 +719,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
-      <c r="B9" s="14"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
@@ -730,7 +730,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
@@ -740,7 +740,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
@@ -750,7 +750,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
-      <c r="B12" s="14"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
@@ -760,7 +760,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
@@ -772,7 +772,7 @@
       <c r="A14" s="11">
         <v>3</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="12">
         <v>45637</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -806,7 +806,7 @@
       <c r="A17" s="11">
         <v>4</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="12">
         <v>45638</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -840,7 +840,7 @@
       <c r="A20" s="11">
         <v>5</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="12">
         <v>45639</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -891,7 +891,7 @@
       <c r="A24" s="11">
         <v>7</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="12">
         <v>45642</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -903,7 +903,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
-      <c r="B25" s="14"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
@@ -916,7 +916,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
-      <c r="B26" s="14"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="1" t="s">
         <v>27</v>
       </c>
@@ -926,7 +926,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
-      <c r="B27" s="14"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="1" t="s">
         <v>28</v>
       </c>
@@ -936,7 +936,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
-      <c r="B28" s="14"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
@@ -946,7 +946,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
-      <c r="B29" s="14"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="1" t="s">
         <v>30</v>
       </c>
@@ -956,7 +956,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
-      <c r="B30" s="14"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="1" t="s">
         <v>31</v>
       </c>
@@ -966,7 +966,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
-      <c r="B31" s="14"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
@@ -976,7 +976,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
-      <c r="B32" s="14"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="1" t="s">
         <v>33</v>
       </c>
@@ -986,7 +986,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
-      <c r="B33" s="14"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="1" t="s">
         <v>34</v>
       </c>
@@ -996,7 +996,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
-      <c r="B34" s="14"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="1" t="s">
         <v>35</v>
       </c>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
-      <c r="B35" s="14"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="1" t="s">
         <v>36</v>
       </c>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
-      <c r="B36" s="14"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="1" t="s">
         <v>37</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="A37" s="11">
         <v>8</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="12">
         <v>45643</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1040,7 +1040,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
-      <c r="B38" s="14"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="1" t="s">
         <v>39</v>
       </c>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="11"/>
-      <c r="B39" s="14"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="1" t="s">
         <v>40</v>
       </c>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="11"/>
-      <c r="B40" s="14"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="11"/>
-      <c r="B41" s="14"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="1" t="s">
         <v>42</v>
       </c>
@@ -1082,7 +1082,7 @@
       <c r="A42" s="11">
         <v>9</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="12">
         <v>45644</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1094,7 +1094,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="11"/>
-      <c r="B43" s="14"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="1" t="s">
         <v>43</v>
       </c>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>
-      <c r="B44" s="14"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="1" t="s">
         <v>41</v>
       </c>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="11"/>
-      <c r="B45" s="14"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="1" t="s">
         <v>44</v>
       </c>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="11"/>
-      <c r="B46" s="14"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="1" t="s">
         <v>45</v>
       </c>
@@ -1136,7 +1136,7 @@
       <c r="A47" s="11">
         <v>10</v>
       </c>
-      <c r="B47" s="14">
+      <c r="B47" s="12">
         <v>45645</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1148,7 +1148,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11"/>
-      <c r="B48" s="14"/>
+      <c r="B48" s="12"/>
       <c r="C48" s="3" t="s">
         <v>46</v>
       </c>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="49" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11"/>
-      <c r="B49" s="14"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="8" t="s">
         <v>47</v>
       </c>
@@ -1170,7 +1170,7 @@
       <c r="A50" s="11">
         <v>11</v>
       </c>
-      <c r="B50" s="14">
+      <c r="B50" s="12">
         <v>45646</v>
       </c>
       <c r="C50" s="9" t="s">
@@ -1182,7 +1182,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="11"/>
-      <c r="B51" s="14"/>
+      <c r="B51" s="12"/>
       <c r="C51" t="s">
         <v>50</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="A52" s="11">
         <v>12</v>
       </c>
-      <c r="B52" s="14">
+      <c r="B52" s="12">
         <v>45649</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -1232,7 +1232,7 @@
       <c r="A55" s="11">
         <v>14</v>
       </c>
-      <c r="B55" s="14">
+      <c r="B55" s="12">
         <v>45652</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -1280,7 +1280,7 @@
       <c r="A59" s="11">
         <v>16</v>
       </c>
-      <c r="B59" s="14">
+      <c r="B59" s="12">
         <v>45656</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -1304,7 +1304,7 @@
       <c r="A61" s="11">
         <v>17</v>
       </c>
-      <c r="B61" s="12">
+      <c r="B61" s="14">
         <v>45657</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -1316,7 +1316,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="11"/>
-      <c r="B62" s="13"/>
+      <c r="B62" s="15"/>
       <c r="C62" s="1" t="s">
         <v>56</v>
       </c>
@@ -1342,7 +1342,7 @@
       <c r="A64" s="11">
         <v>19</v>
       </c>
-      <c r="B64" s="14">
+      <c r="B64" s="12">
         <v>45659</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -1400,7 +1400,7 @@
       <c r="A69" s="11">
         <v>21</v>
       </c>
-      <c r="B69" s="14">
+      <c r="B69" s="12">
         <v>45663</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -1412,7 +1412,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="11"/>
-      <c r="B70" s="14"/>
+      <c r="B70" s="12"/>
       <c r="C70" s="1" t="s">
         <v>64</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="A71" s="11">
         <v>22</v>
       </c>
-      <c r="B71" s="14">
+      <c r="B71" s="12">
         <v>45664</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -1450,8 +1450,55 @@
         <v>69</v>
       </c>
     </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="11">
+        <v>23</v>
+      </c>
+      <c r="B73" s="12">
+        <v>45665</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D73" t="s">
+        <v>68</v>
+      </c>
+      <c r="E73" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D74" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="36">
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="A24:A36"/>
+    <mergeCell ref="B24:B36"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="B69:B70"/>
     <mergeCell ref="A71:A72"/>
@@ -1468,24 +1515,6 @@
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="A55:A57"/>
     <mergeCell ref="B55:B57"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="A24:A36"/>
-    <mergeCell ref="B24:B36"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E25" r:id="rId1" display="https://github.com/Swathiloya/Daily_Status" xr:uid="{C3116F7F-791E-4165-A1F6-266C944CBF68}"/>

</xml_diff>